<commit_message>
added exact strings from TSETMC
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -923,6 +923,354 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>بازار ابزارهاي نوين مالي فرابورس</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>IFB.NFinTools</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>بازار پايه زرد فرابورس</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>IFB.Paye.Yellow</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>بازار پايه زرد فرابورس قانون احکام دائمی برنامه های توسعه کشور</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>IFB.Paye.Yellow</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>بازار اول (تابلوي اصلي) بورس</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>TSE.M1.Main</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>بازار اول (تابلوي فرعي) بورس</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>TSE.M1.Subsidiary</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>بازار پايه نارنجي فرابورس</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>IFB.Paye.Orange</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>بازار ابزارهاي مشتقه فرابورس</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>IFB.Derivatives</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>بازار اوراق بدهي</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>TSE.Bonds</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>بازار پايه زرد فرابورس لغو پذیرش شده</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>IFB.Paye.Yellow</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>بازار پايه نارنجي فرابورس لغو پذیرش شده</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>IFB.Paye.Orange</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>بازار پايه قرمز فرابورس قانون احکام دائمی برنامه های توسعه کشور</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>IFB.Paye.Red</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>بازار سوم فرابورس قانون احکام دائمی برنامه های توسعه کشور</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>IFB.M3</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>بازار پايه قرمز فرابورس قانون احکام دائمی برنامه های توسعه کشور/ اظهارنظر مردود</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>IFB.Paye.Red</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>بازار عادي آتي</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>TSE.Derivatives</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>بازار پايه نارنجي فرابورس قانون احکام دائمی برنامه های توسعه کشور/عدم اظهارنظر</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>IFB.Paye.Orange</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>بازار ابزارهاي مشتقه</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>IFB.Derivatives</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>بازار پايه نارنجي فرابورس لغو پذیرش شده/ اظهارنظر مردود</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>IFB.Paye.Orange</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>بازار پايه قرمز فرابورس لغو پذیرش شده/اظهارنظر مردود</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>IFB.Paye.Red</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>بازار پايه نارنجي فرابورس لغو پذیرش شده/عدم اظهارنظر</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>IFB.Paye.Orange</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>بازار پايه  فرابورس</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>IFB.Paye</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>شرکتهاي کوچک و متوسط فرابورس</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>IFB.SME</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>بازار پايه قرمز فرابورس</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>IFB.Paye.Red</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>بازار پايه قرمز فرابورس لغو پذیرش شده/عدم اظهارنظر/ورشکستگی</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>IFB.Paye.Red</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>بازار دوم فرابورس قانون احکام دائمی برنامه های توسعه کشور</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>IFB.M2</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>بازار پايه نارنجي فرابورس قانون احکام دائمی برنامه های توسعه کشور</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>IFB.Paye.Orange</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>بازار پايه  فرابورس قانون احکام دائمی برنامه های توسعه کشور</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>IFB.Paye</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>بازار پايه نارنجي فرابورس لغو پذیرش شده/ عدم اظهارنظر</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>IFB.Paye.Orange</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>بازار پايه قرمز فرابورس لغو پذیرش شده/ عدم اظهارنظر/ انحلال</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>IFB.Paye.Red</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>بازار پايه قرمز فرابورس لغو پذیرش شده</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>IFB.Paye.Red</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
sorted by repo: https://github.com/imahdimir/gov-d-MarketTitle-2-MarketId
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -475,7 +475,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>بازار ابزارهای مشتقه</t>
+          <t>بازار ابزارهاي مشتقه</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -487,7 +487,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>بازار ابزارهای مشتقه فرابورس</t>
+          <t>بازار ابزارهاي مشتقه فرابورس</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -499,55 +499,55 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>بازار اول فرابورس</t>
+          <t>بازار ابزارهای مشتقه</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>IFB.M1</t>
+          <t>IFB.Derivatives</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>بازار اول فرابورس لغو پذیرش شده</t>
+          <t>بازار ابزارهای مشتقه فرابورس</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>IFB.M1</t>
+          <t>IFB.Derivatives</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>بازار دوم فرابورس</t>
+          <t>بازار اول فرابورس</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>IFB.M2</t>
+          <t>IFB.M1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>بازار دوم فرابورس قانون احکام دایمی برنامه های توسعه کشور</t>
+          <t>بازار اول فرابورس لغو پذیرش شده</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>IFB.M2</t>
+          <t>IFB.M1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>بازار دوم فرابورس لغو پذیرش شده</t>
+          <t>بازار دوم فرابورس</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -559,715 +559,715 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>بازار سوم فرابورس</t>
+          <t>بازار دوم فرابورس قانون احکام دائمی برنامه های توسعه کشور</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>IFB.M3</t>
+          <t>IFB.M2</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>بازار سوم فرابورس قانون احکام دایمی برنامه های توسعه کشور</t>
+          <t>بازار دوم فرابورس قانون احکام دایمی برنامه های توسعه کشور</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>IFB.M3</t>
+          <t>IFB.M2</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>بازار ابزارهای نوین مالی فرابورس</t>
+          <t>بازار دوم فرابورس لغو پذیرش شده</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>IFB.NFinTools</t>
+          <t>IFB.M2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>بازار پایه فرابورس</t>
+          <t>بازار سوم فرابورس</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>IFB.Paye</t>
+          <t>IFB.M3</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>بازار پایه فرابورس قانون احکام دایمی برنامه های توسعه کشور</t>
+          <t>بازار سوم فرابورس قانون احکام دائمی برنامه های توسعه کشور</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>IFB.Paye</t>
+          <t>IFB.M3</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>بازار پایه نارنجی فرابورس</t>
+          <t>بازار سوم فرابورس قانون احکام دایمی برنامه های توسعه کشور</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>IFB.Paye.Orange</t>
+          <t>IFB.M3</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>بازار پایه نارنجی فرابورس قانون احکام دایمی برنامه های توسعه کشور</t>
+          <t>بازار ابزارهاي نوين مالي فرابورس</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>IFB.Paye.Orange</t>
+          <t>IFB.NFinTools</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>بازار پایه نارنجی فرابورس قانون احکام دایمی برنامه های توسعه کشور/عدم اظهارنظر</t>
+          <t>بازار ابزارهای نوین مالی فرابورس</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>IFB.Paye.Orange</t>
+          <t>IFB.NFinTools</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>بازار پایه نارنجی فرابورس لغو پذیرش شده</t>
+          <t>بازار پايه  فرابورس</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>IFB.Paye.Orange</t>
+          <t>IFB.Paye</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>بازار پایه نارنجی فرابورس لغو پذیرش شده/ اظهارنظر مردود</t>
+          <t>بازار پايه  فرابورس قانون احکام دائمی برنامه های توسعه کشور</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>IFB.Paye.Orange</t>
+          <t>IFB.Paye</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>بازار پایه نارنجی فرابورس لغو پذیرش شده/ عدم اظهارنظر</t>
+          <t>بازار پایه فرابورس</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>IFB.Paye.Orange</t>
+          <t>IFB.Paye</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>بازار پایه نارنجی فرابورس لغو پذیرش شده/عدم اظهارنظر</t>
+          <t>بازار پایه فرابورس قانون احکام دایمی برنامه های توسعه کشور</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>IFB.Paye.Orange</t>
+          <t>IFB.Paye</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>بازار پایه قرمز فرابورس</t>
+          <t>بازار پايه نارنجي فرابورس</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>IFB.Paye.Red</t>
+          <t>IFB.Paye.Orange</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>بازار پایه قرمز فرابورس قانون احکام دایمی برنامه های توسعه کشور</t>
+          <t>بازار پايه نارنجي فرابورس قانون احکام دائمی برنامه های توسعه کشور</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>IFB.Paye.Red</t>
+          <t>IFB.Paye.Orange</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>بازار پایه قرمز فرابورس قانون احکام دایمی برنامه های توسعه کشور/ اظهارنظر مردود</t>
+          <t>بازار پايه نارنجي فرابورس قانون احکام دائمی برنامه های توسعه کشور/عدم اظهارنظر</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>IFB.Paye.Red</t>
+          <t>IFB.Paye.Orange</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>بازار پایه قرمز فرابورس لغو پذیرش شده</t>
+          <t>بازار پايه نارنجي فرابورس لغو پذیرش شده</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>IFB.Paye.Red</t>
+          <t>IFB.Paye.Orange</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>بازار پایه قرمز فرابورس لغو پذیرش شده/ عدم اظهارنظر/ انحلال</t>
+          <t>بازار پايه نارنجي فرابورس لغو پذیرش شده/ اظهارنظر مردود</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>IFB.Paye.Red</t>
+          <t>IFB.Paye.Orange</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>بازار پایه قرمز فرابورس لغو پذیرش شده/اظهارنظر مردود</t>
+          <t>بازار پايه نارنجي فرابورس لغو پذیرش شده/ عدم اظهارنظر</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>IFB.Paye.Red</t>
+          <t>IFB.Paye.Orange</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>بازار پایه قرمز فرابورس لغو پذیرش شده/عدم اظهارنظر/ورشکستگی</t>
+          <t>بازار پايه نارنجي فرابورس لغو پذیرش شده/عدم اظهارنظر</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>IFB.Paye.Red</t>
+          <t>IFB.Paye.Orange</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>بازار پایه زرد فرابورس</t>
+          <t>بازار پایه نارنجی فرابورس</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>IFB.Paye.Yellow</t>
+          <t>IFB.Paye.Orange</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>بازار پایه زرد فرابورس قانون احکام دایمی برنامه های توسعه کشور</t>
+          <t>بازار پایه نارنجی فرابورس قانون احکام دایمی برنامه های توسعه کشور</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>IFB.Paye.Yellow</t>
+          <t>IFB.Paye.Orange</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>بازار پایه زرد فرابورس لغو پذیرش شده</t>
+          <t>بازار پایه نارنجی فرابورس قانون احکام دایمی برنامه های توسعه کشور/عدم اظهارنظر</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>IFB.Paye.Yellow</t>
+          <t>IFB.Paye.Orange</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>شرکتهای کوچک و متوسط فرابورس</t>
+          <t>بازار پایه نارنجی فرابورس لغو پذیرش شده</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>IFB.SME</t>
+          <t>IFB.Paye.Orange</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>بورس کالا</t>
+          <t>بازار پایه نارنجی فرابورس لغو پذیرش شده/ اظهارنظر مردود</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>IME</t>
+          <t>IFB.Paye.Orange</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>بازار اوراق بدهی</t>
+          <t>بازار پایه نارنجی فرابورس لغو پذیرش شده/ عدم اظهارنظر</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>TSE.Bonds</t>
+          <t>IFB.Paye.Orange</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>بازار عادی آتی</t>
+          <t>بازار پایه نارنجی فرابورس لغو پذیرش شده/عدم اظهارنظر</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>TSE.Derivatives</t>
+          <t>IFB.Paye.Orange</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>بازار اول (تابلوی اصلی) بورس</t>
+          <t>بازار پايه قرمز فرابورس</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>TSE.M1.Main</t>
+          <t>IFB.Paye.Red</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>بازار اول (تابلوی فرعی) بورس</t>
+          <t>بازار پايه قرمز فرابورس قانون احکام دائمی برنامه های توسعه کشور</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>TSE.M1.Subsidiary</t>
+          <t>IFB.Paye.Red</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>بازار دوم بورس</t>
+          <t>بازار پايه قرمز فرابورس قانون احکام دائمی برنامه های توسعه کشور/ اظهارنظر مردود</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>TSE.M2</t>
+          <t>IFB.Paye.Red</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>بازار چهارم بورس</t>
+          <t>بازار پايه قرمز فرابورس لغو پذیرش شده</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>TSE.M4</t>
+          <t>IFB.Paye.Red</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>لغو پذیرش شده</t>
+          <t>بازار پايه قرمز فرابورس لغو پذیرش شده/ عدم اظهارنظر/ انحلال</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>IFB.Paye.Red</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>بازار ابزارهاي نوين مالي فرابورس</t>
+          <t>بازار پايه قرمز فرابورس لغو پذیرش شده/اظهارنظر مردود</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>IFB.NFinTools</t>
+          <t>IFB.Paye.Red</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>بازار پايه زرد فرابورس</t>
+          <t>بازار پايه قرمز فرابورس لغو پذیرش شده/عدم اظهارنظر/ورشکستگی</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>IFB.Paye.Yellow</t>
+          <t>IFB.Paye.Red</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>بازار پايه زرد فرابورس قانون احکام دائمی برنامه های توسعه کشور</t>
+          <t>بازار پایه قرمز فرابورس</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>IFB.Paye.Yellow</t>
+          <t>IFB.Paye.Red</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>بازار اول (تابلوي اصلي) بورس</t>
+          <t>بازار پایه قرمز فرابورس قانون احکام دایمی برنامه های توسعه کشور</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>TSE.M1.Main</t>
+          <t>IFB.Paye.Red</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>بازار اول (تابلوي فرعي) بورس</t>
+          <t>بازار پایه قرمز فرابورس قانون احکام دایمی برنامه های توسعه کشور/ اظهارنظر مردود</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>TSE.M1.Subsidiary</t>
+          <t>IFB.Paye.Red</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>بازار پايه نارنجي فرابورس</t>
+          <t>بازار پایه قرمز فرابورس لغو پذیرش شده</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>IFB.Paye.Orange</t>
+          <t>IFB.Paye.Red</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>بازار ابزارهاي مشتقه فرابورس</t>
+          <t>بازار پایه قرمز فرابورس لغو پذیرش شده/ عدم اظهارنظر/ انحلال</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>IFB.Derivatives</t>
+          <t>IFB.Paye.Red</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>بازار اوراق بدهي</t>
+          <t>بازار پایه قرمز فرابورس لغو پذیرش شده/اظهارنظر مردود</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>TSE.Bonds</t>
+          <t>IFB.Paye.Red</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>بازار پايه زرد فرابورس لغو پذیرش شده</t>
+          <t>بازار پایه قرمز فرابورس لغو پذیرش شده/عدم اظهارنظر/ورشکستگی</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>IFB.Paye.Yellow</t>
+          <t>IFB.Paye.Red</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>بازار پايه نارنجي فرابورس لغو پذیرش شده</t>
+          <t>بازار پايه زرد فرابورس</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>IFB.Paye.Orange</t>
+          <t>IFB.Paye.Yellow</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>بازار پايه قرمز فرابورس قانون احکام دائمی برنامه های توسعه کشور</t>
+          <t>بازار پايه زرد فرابورس قانون احکام دائمی برنامه های توسعه کشور</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>IFB.Paye.Red</t>
+          <t>IFB.Paye.Yellow</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>بازار سوم فرابورس قانون احکام دائمی برنامه های توسعه کشور</t>
+          <t>بازار پايه زرد فرابورس لغو پذیرش شده</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>IFB.M3</t>
+          <t>IFB.Paye.Yellow</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>بازار پايه قرمز فرابورس قانون احکام دائمی برنامه های توسعه کشور/ اظهارنظر مردود</t>
+          <t>بازار پایه زرد فرابورس</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>IFB.Paye.Red</t>
+          <t>IFB.Paye.Yellow</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>بازار عادي آتي</t>
+          <t>بازار پایه زرد فرابورس قانون احکام دایمی برنامه های توسعه کشور</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>TSE.Derivatives</t>
+          <t>IFB.Paye.Yellow</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>بازار پايه نارنجي فرابورس قانون احکام دائمی برنامه های توسعه کشور/عدم اظهارنظر</t>
+          <t>بازار پایه زرد فرابورس لغو پذیرش شده</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>IFB.Paye.Orange</t>
+          <t>IFB.Paye.Yellow</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>بازار ابزارهاي مشتقه</t>
+          <t>شرکتهاي کوچک و متوسط فرابورس</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>IFB.Derivatives</t>
+          <t>IFB.SME</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>بازار پايه نارنجي فرابورس لغو پذیرش شده/ اظهارنظر مردود</t>
+          <t>شرکتهای کوچک و متوسط فرابورس</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>IFB.Paye.Orange</t>
+          <t>IFB.SME</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>بازار پايه قرمز فرابورس لغو پذیرش شده/اظهارنظر مردود</t>
+          <t>بورس کالا</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>IFB.Paye.Red</t>
+          <t>IME</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>بازار پايه نارنجي فرابورس لغو پذیرش شده/عدم اظهارنظر</t>
+          <t>بازار اوراق بدهي</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>IFB.Paye.Orange</t>
+          <t>TSE.Bonds</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>بازار پايه  فرابورس</t>
+          <t>بازار اوراق بدهی</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>IFB.Paye</t>
+          <t>TSE.Bonds</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>شرکتهاي کوچک و متوسط فرابورس</t>
+          <t>بازار عادي آتي</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>IFB.SME</t>
+          <t>TSE.Derivatives</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>بازار پايه قرمز فرابورس</t>
+          <t>بازار عادی آتی</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>IFB.Paye.Red</t>
+          <t>TSE.Derivatives</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>بازار پايه قرمز فرابورس لغو پذیرش شده/عدم اظهارنظر/ورشکستگی</t>
+          <t>بازار اول (تابلوي اصلي) بورس</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>IFB.Paye.Red</t>
+          <t>TSE.M1.Main</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>بازار دوم فرابورس قانون احکام دائمی برنامه های توسعه کشور</t>
+          <t>بازار اول (تابلوی اصلی) بورس</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>IFB.M2</t>
+          <t>TSE.M1.Main</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>بازار پايه نارنجي فرابورس قانون احکام دائمی برنامه های توسعه کشور</t>
+          <t>بازار اول (تابلوي فرعي) بورس</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>IFB.Paye.Orange</t>
+          <t>TSE.M1.Subsidiary</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>بازار پايه  فرابورس قانون احکام دائمی برنامه های توسعه کشور</t>
+          <t>بازار اول (تابلوی فرعی) بورس</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>IFB.Paye</t>
+          <t>TSE.M1.Subsidiary</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>بازار پايه نارنجي فرابورس لغو پذیرش شده/ عدم اظهارنظر</t>
+          <t>بازار دوم بورس</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>IFB.Paye.Orange</t>
+          <t>TSE.M2</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>بازار پايه قرمز فرابورس لغو پذیرش شده/ عدم اظهارنظر/ انحلال</t>
+          <t>بازار چهارم بورس</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>IFB.Paye.Red</t>
+          <t>TSE.M4</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>بازار پايه قرمز فرابورس لغو پذیرش شده</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>IFB.Paye.Red</t>
+          <t>لغو پذیرش شده</t>
         </is>
       </c>
     </row>

</xml_diff>